<commit_message>
Update MCDA default weights and ranges
</commit_message>
<xml_diff>
--- a/data-raw/mcda-defaults.xlsx
+++ b/data-raw/mcda-defaults.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14620" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="3-state" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="21">
   <si>
     <t>criteria_name</t>
   </si>
@@ -43,9 +43,6 @@
     <t>Loss of income</t>
   </si>
   <si>
-    <t>Aes combined</t>
-  </si>
-  <si>
     <t>Administered orally</t>
   </si>
   <si>
@@ -56,6 +53,36 @@
   </si>
   <si>
     <t>max</t>
+  </si>
+  <si>
+    <t>Elevated alanine transaminase</t>
+  </si>
+  <si>
+    <t>Elevated aspartate transaminase</t>
+  </si>
+  <si>
+    <t>Diarrhea</t>
+  </si>
+  <si>
+    <t>Dry skin</t>
+  </si>
+  <si>
+    <t>Eye problems</t>
+  </si>
+  <si>
+    <t>Paronychia</t>
+  </si>
+  <si>
+    <t>Pneumonitis</t>
+  </si>
+  <si>
+    <t>Pruritis</t>
+  </si>
+  <si>
+    <t>Rash</t>
+  </si>
+  <si>
+    <t>Stomatitis</t>
   </si>
 </sst>
 </file>
@@ -104,17 +131,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -444,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -460,13 +500,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>10</v>
-      </c>
-      <c r="D1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -515,7 +555,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -557,15 +597,151 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>5</v>
+        <v>11</v>
+      </c>
+      <c r="B8" s="1">
+        <f>5/10</f>
+        <v>0.5</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>0.26</v>
       </c>
       <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1">
+        <f t="shared" ref="B9:B17" si="0">5/10</f>
+        <v>0.5</v>
+      </c>
+      <c r="C9">
+        <v>0.2</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="1">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="C10">
+        <v>0.3</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="1">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="C11">
+        <v>0.03</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="1">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="C12">
+        <v>0.02</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="1">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="C13">
+        <v>0.1</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="1">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="C14">
+        <v>0.06</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="1">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="C15">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="1">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="C16">
+        <v>0.65</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="1">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="C17">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D17">
         <v>0</v>
       </c>
     </row>
@@ -581,15 +757,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="A9:D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="1"/>
     <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.6640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -598,21 +775,21 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>10</v>
-      </c>
-      <c r="D1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>10</v>
       </c>
       <c r="C2">
@@ -627,7 +804,7 @@
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>10</v>
       </c>
       <c r="C3">
@@ -642,7 +819,7 @@
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>10</v>
       </c>
       <c r="C4">
@@ -657,7 +834,7 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>5</v>
       </c>
       <c r="C5">
@@ -669,9 +846,9 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1">
         <v>0</v>
       </c>
       <c r="C6">
@@ -685,7 +862,7 @@
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>0</v>
       </c>
       <c r="C7">
@@ -699,7 +876,7 @@
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>0</v>
       </c>
       <c r="C8">
@@ -711,15 +888,151 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>5</v>
+        <v>11</v>
+      </c>
+      <c r="B9" s="1">
+        <f>5/10</f>
+        <v>0.5</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>0.26</v>
       </c>
       <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="1">
+        <f t="shared" ref="B10:B18" si="0">5/10</f>
+        <v>0.5</v>
+      </c>
+      <c r="C10">
+        <v>0.2</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="1">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="C11">
+        <v>0.3</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="1">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="C12">
+        <v>0.03</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="1">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="C13">
+        <v>0.02</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="1">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="C14">
+        <v>0.1</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="1">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="C15">
+        <v>0.06</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="1">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="C16">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="1">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="C17">
+        <v>0.65</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="1">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="C18">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D18">
         <v>0</v>
       </c>
     </row>

</xml_diff>